<commit_message>
Created UI based on the wireframe.
Created and added the MainWindow.fxml code to display the UI that is
shown in the wireframe.
Updated the MainWindow.java code to reflect the added fxml elements to
the view.
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog Burndown.xlsx
+++ b/documentation/Sprint Backlog Burndown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcorley\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/daf4c36fd6410f15/Desktop/JamesBridgesHW5_Sprint1/TextAdventureGame/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C86FA19-BAF0-4882-AC44-363173A7A31F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{2C86FA19-BAF0-4882-AC44-363173A7A31F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45A3F5DB-CA08-4286-B341-007494EB90E1}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24" yWindow="876" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1349,14 +1349,14 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.85546875" customWidth="1"/>
-    <col min="2" max="2" width="41.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1373,7 +1373,7 @@
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -1390,7 +1390,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1405,7 +1405,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>10</v>
@@ -1418,7 +1418,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>11</v>
@@ -1431,7 +1431,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>12</v>
@@ -1444,7 +1444,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>13</v>
@@ -1457,7 +1457,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>14</v>
@@ -1470,7 +1470,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>16</v>
@@ -1483,7 +1483,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1492,7 +1492,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1501,7 +1501,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1510,7 +1510,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1519,7 +1519,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1528,7 +1528,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1537,7 +1537,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1546,7 +1546,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1555,7 +1555,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1564,7 +1564,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1573,7 +1573,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1582,7 +1582,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1591,7 +1591,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1600,7 +1600,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1609,7 +1609,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1618,7 +1618,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1627,7 +1627,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1636,7 +1636,7 @@
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B27" s="4" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Added Player class with basic functionality.
Added Player class that has a 'health' field with getters/setters.
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog Burndown.xlsx
+++ b/documentation/Sprint Backlog Burndown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/daf4c36fd6410f15/Desktop/JamesBridgesHW5_Sprint1/TextAdventureGame/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{2C86FA19-BAF0-4882-AC44-363173A7A31F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45A3F5DB-CA08-4286-B341-007494EB90E1}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{2C86FA19-BAF0-4882-AC44-363173A7A31F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCD214A5-6057-4A23-8CB9-7231783B4B3C}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="876" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3636" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -292,7 +292,7 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1080,6 +1080,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1346,7 +1350,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1400,7 +1404,9 @@
       <c r="C3" s="1">
         <v>1.5</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -1646,7 +1652,7 @@
       </c>
       <c r="D27" s="3">
         <f t="shared" ref="D27:G27" si="0">SUM(D3:D26)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E27" s="3">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Added GameManager class and refactored project.
Added GameManager class:
    fields:
        world:              the game world
        worldManager:       the manager for the game world
        player:             the player of the game
        currentLocation:    the current Location that the player is ActionTest
        isGameOverLose:     flag for if the player loses the game
        isGameOverWin:      flag for if the player wins the game
        gameOverMessage:    the message to be displayed at gameOver

Refactored the following:
    WorldManager:           no longer had the startLcoation field

    Location:               removed the hazardDamage field

    GlobalEnums:            Added PIT to HazardType

    World:                  Added HazardManager reference
                            Moved startLocation reference here

Added/updated test classes
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog Burndown.xlsx
+++ b/documentation/Sprint Backlog Burndown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/daf4c36fd6410f15/Desktop/JamesBridgesHW5_Sprint1/TextAdventureGame/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{2C86FA19-BAF0-4882-AC44-363173A7A31F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCD214A5-6057-4A23-8CB9-7231783B4B3C}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{2C86FA19-BAF0-4882-AC44-363173A7A31F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F97212D0-0B47-4C52-9EB0-2B2588438E3D}"/>
   <bookViews>
-    <workbookView xWindow="3636" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -292,7 +292,7 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1350,7 +1350,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1419,7 +1419,9 @@
       <c r="C4" s="1">
         <v>2</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1432,7 +1434,9 @@
       <c r="C5" s="1">
         <v>0.5</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1445,7 +1449,9 @@
       <c r="C6" s="1">
         <v>2</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -1458,7 +1464,9 @@
       <c r="C7" s="1">
         <v>4</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1471,7 +1479,9 @@
       <c r="C8" s="1">
         <v>3.5</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1484,7 +1494,9 @@
       <c r="C9" s="1">
         <v>0.5</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -1652,7 +1664,7 @@
       </c>
       <c r="D27" s="3">
         <f t="shared" ref="D27:G27" si="0">SUM(D3:D26)</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E27" s="3">
         <f t="shared" si="0"/>

</xml_diff>